<commit_message>
new file:   Eligible Merger/Eligible.py modified:   Eligible Merger/Eligibles.xlsx modified:   Eligible Merger/companies.xlsx modified:   Extractor/companies.txt modified:   Extractor/companies.xlsx modified:   Extractor/details.xlsx modified:   Merger/details.xlsx modified:   main.py
</commit_message>
<xml_diff>
--- a/Eligible Merger/Eligibles.xlsx
+++ b/Eligible Merger/Eligibles.xlsx
@@ -1347,10 +1347,10 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:L9"/>
+  <dimension ref="A1:L15"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E18" sqref="E18"/>
+      <selection activeCell="E16" sqref="E15:E16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.14285714285714" defaultRowHeight="15"/>
@@ -1549,6 +1549,14 @@
       <c r="I9"/>
       <c r="L9"/>
     </row>
+    <row r="10" spans="1:1">
+      <c r="A10"/>
+    </row>
+    <row r="15" spans="8:12">
+      <c r="H15"/>
+      <c r="I15"/>
+      <c r="L15"/>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <headerFooter/>

</xml_diff>